<commit_message>
editing sheet of dataset features
</commit_message>
<xml_diff>
--- a/datasets/compas-propublica/compas-scores-two-years - atributos e descrições.xlsx
+++ b/datasets/compas-propublica/compas-scores-two-years - atributos e descrições.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Downloads\Temporario\fairness-testing\datasets\compas-propublica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02083745-A0F1-441E-97B2-562574A7BA58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6C2146D-8FDF-4F4B-AD98-A4C2A0C2E23A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="110">
   <si>
     <t>Atributos Dataset COMPAS</t>
   </si>
@@ -340,6 +340,21 @@
   </si>
   <si>
     <t>custody_days</t>
+  </si>
+  <si>
+    <t>índices das variáveis categóricas</t>
+  </si>
+  <si>
+    <t>sex = {'Female':1, 'Male':2}</t>
+  </si>
+  <si>
+    <t>race = {'African-American':1, 'Asian':2, 'Caucasian':3, 'Hispanic':4, 'Native American':5, 'Other':6}</t>
+  </si>
+  <si>
+    <t>c_charge_degree = {'F':1, 'M':2}</t>
+  </si>
+  <si>
+    <t>r_vr_charge_degree = {np.nan:0, '(CO3)':1, '(F1)':2, '(F2)':3, '(F3)':4, '(F5)':5, '(F6)':6, '(F7)':7, '(M1)':8, '(M2)':9, '(MO3)':10}</t>
   </si>
 </sst>
 </file>
@@ -741,6 +756,7 @@
   <cols>
     <col min="2" max="2" width="25" style="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="76.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="109.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
@@ -800,6 +816,9 @@
       <c r="C7" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="F7" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
@@ -808,6 +827,9 @@
       <c r="C8" s="3" t="s">
         <v>56</v>
       </c>
+      <c r="F8" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
@@ -816,6 +838,9 @@
       <c r="C9" s="2" t="s">
         <v>57</v>
       </c>
+      <c r="F9" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
@@ -824,6 +849,9 @@
       <c r="C10" s="3" t="s">
         <v>58</v>
       </c>
+      <c r="F10" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
@@ -831,6 +859,9 @@
       </c>
       <c r="C11" s="3" t="s">
         <v>59</v>
+      </c>
+      <c r="F11" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">

</xml_diff>